<commit_message>
Integrated Recomendation Engine with REST API
</commit_message>
<xml_diff>
--- a/major_rec/majors.xlsx
+++ b/major_rec/majors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berk/code/hackathon/major_rec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D356AF-6663-3445-9B94-B469B60D0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F451A8-3B34-4346-9A0C-F417776AE8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="0" windowWidth="21880" windowHeight="21000" xr2:uid="{C1FE8DAC-07FD-3948-BCB1-EBB5FAAD3FD6}"/>
+    <workbookView xWindow="11720" yWindow="500" windowWidth="21880" windowHeight="19080" xr2:uid="{C1FE8DAC-07FD-3948-BCB1-EBB5FAAD3FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="148">
   <si>
     <t>Biology</t>
   </si>
@@ -414,9 +414,6 @@
     <t>ENG 494 - Special Topics in Linguistics (3 units: C- or better)</t>
   </si>
   <si>
-    <t>Humanities, Social Sciences</t>
-  </si>
-  <si>
     <t>ENG 210 - Introduction to Language and Linguistics (3 units: C- or better)</t>
   </si>
   <si>
@@ -472,6 +469,15 @@
   </si>
   <si>
     <t>Pre 1600 History</t>
+  </si>
+  <si>
+    <t>Physics, Chemistry</t>
+  </si>
+  <si>
+    <t>Physical Chemistry</t>
+  </si>
+  <si>
+    <t>Engineering, Physics</t>
   </si>
 </sst>
 </file>
@@ -838,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3871CD39-76CE-3949-8936-7BD716B158C2}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +952,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -976,7 +982,7 @@
         <v>76</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>21</v>
@@ -1259,7 +1265,7 @@
         <v>52</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>58</v>
@@ -1380,7 +1386,7 @@
         <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>19</v>
@@ -1410,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>87</v>
@@ -1436,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>21</v>
@@ -1472,7 +1478,7 @@
         <v>19</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>87</v>
@@ -1489,7 +1495,7 @@
         <v>121</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>123</v>
@@ -1501,16 +1507,16 @@
         <v>125</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>22</v>
@@ -1522,7 +1528,7 @@
         <v>64</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>87</v>
@@ -1534,7 +1540,7 @@
         <v>12</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>21</v>
@@ -1551,7 +1557,7 @@
         <v>122</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>124</v>
@@ -1560,22 +1566,22 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>69</v>
@@ -1584,28 +1590,28 @@
         <v>77</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="P12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="Q12" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modified training data for environmental science
</commit_message>
<xml_diff>
--- a/major_rec/majors.xlsx
+++ b/major_rec/majors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berk/code/hackathon/major_rec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F451A8-3B34-4346-9A0C-F417776AE8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB2573-6B29-2B42-85C8-E0108969E323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="500" windowWidth="21880" windowHeight="19080" xr2:uid="{C1FE8DAC-07FD-3948-BCB1-EBB5FAAD3FD6}"/>
+    <workbookView xWindow="11720" yWindow="500" windowWidth="21880" windowHeight="19020" xr2:uid="{C1FE8DAC-07FD-3948-BCB1-EBB5FAAD3FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="150">
   <si>
     <t>Biology</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Engineering, Physics</t>
+  </si>
+  <si>
+    <t>Biology, Environmental Science</t>
+  </si>
+  <si>
+    <t>Humanities, Engineering</t>
   </si>
 </sst>
 </file>
@@ -844,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3871CD39-76CE-3949-8936-7BD716B158C2}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,7 +1085,7 @@
         <v>46</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>55</v>
@@ -1247,7 +1253,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>27</v>
@@ -1513,7 +1519,7 @@
         <v>128</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>130</v>

</xml_diff>